<commit_message>
Update per Jim's review
These documents are updated per Jim's review and the Parts List has been
updated with the new, thinner box that Jim found.
</commit_message>
<xml_diff>
--- a/SISHubPartsList.xlsx
+++ b/SISHubPartsList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="103">
   <si>
     <t>Item #</t>
   </si>
@@ -150,15 +150,6 @@
     <t>40 conductor female-female jumper wires, separable.</t>
   </si>
   <si>
-    <t>Office Max</t>
-  </si>
-  <si>
-    <t>enclosure; 1.75 liter (3"H x 7"W x 9-1/2"D)</t>
-  </si>
-  <si>
-    <t>http://www.officedepot.com/a/products/452333/Really-Useful-Boxes-Plastic-Storage-Box/</t>
-  </si>
-  <si>
     <t>A smaller enclosure may be used if receivers are mounted to PC Bord directly vs taped to the sides of the enclosure.  However, range of reception may sugger if the receivers are not at least 4" apart (and apart from the Photon WiFi chip).  Boxes are available is various colors.</t>
   </si>
   <si>
@@ -322,6 +313,18 @@
   </si>
   <si>
     <t>SIS Hub Printed Circuit Board</t>
+  </si>
+  <si>
+    <t>http://www.reallyusefulproducts.co.uk/usa/html/onlineshop/rub/b00_55litre.php</t>
+  </si>
+  <si>
+    <t>enclosure; 0.55 liter (1-7/16"H x 4"W x 8-1/2"L)</t>
+  </si>
+  <si>
+    <t>Staples or on-line from Really Useful Boxes</t>
+  </si>
+  <si>
+    <t>in-store only</t>
   </si>
 </sst>
 </file>
@@ -724,10 +727,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -743,7 +749,7 @@
     <row r="1" spans="1:7">
       <c r="A1" s="9"/>
       <c r="F1" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -778,16 +784,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>42</v>
@@ -814,7 +820,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30">
@@ -832,7 +838,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>38</v>
@@ -847,19 +853,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60">
@@ -871,19 +877,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45">
@@ -907,7 +913,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
@@ -922,13 +928,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>34</v>
@@ -946,16 +952,16 @@
         <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
@@ -973,7 +979,7 @@
         <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>35</v>
@@ -1021,7 +1027,7 @@
         <v>41</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45">
@@ -1039,13 +1045,13 @@
         <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45">
@@ -1057,19 +1063,19 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="G15" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30">
@@ -1093,7 +1099,7 @@
         <v>20</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1101,7 +1107,7 @@
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="F18" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
@@ -1112,19 +1118,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D19" s="8">
-        <v>25038085</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="75">
@@ -1136,19 +1142,19 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75">
@@ -1160,19 +1166,19 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="51.75" customHeight="1">
@@ -1184,19 +1190,19 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="66" customHeight="1">
@@ -1208,19 +1214,19 @@
         <v>100</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30">
@@ -1280,19 +1286,19 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" s="4">
         <v>912408</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30">
@@ -1307,16 +1313,16 @@
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="34.5" customHeight="1">
@@ -1331,16 +1337,16 @@
         <v>13</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1381,7 +1387,7 @@
     <hyperlink ref="F3" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup scale="51" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>